<commit_message>
Docs -> spec technique
</commit_message>
<xml_diff>
--- a/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
+++ b/Documentation/Ecrit/01b_Diagramme_de_Gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programme\wamp64\www\M2L_note_de_frais\Documentation\Ecrit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE1497B-BF47-4CA8-B172-AE7777957A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F37399-AFA4-42FA-959E-09483FB12D17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -924,7 +924,7 @@
   <dimension ref="A1:AK1026"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="F1" s="5">
         <f ca="1">TODAY()</f>
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="7"/>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="E6" s="29">
         <f>(E7+E8)/2</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="17" t="s">
@@ -1338,7 +1338,7 @@
       <c r="L6" s="52"/>
       <c r="M6" s="55">
         <f>$E$6</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="N6" s="55"/>
       <c r="O6" s="55"/>
@@ -1433,7 +1433,7 @@
         <v>63</v>
       </c>
       <c r="E8" s="25">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>37</v>
@@ -1448,7 +1448,7 @@
       <c r="L8" s="52"/>
       <c r="M8" s="55">
         <f>$E$8</f>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N8" s="55"/>
       <c r="O8" s="55"/>

</xml_diff>